<commit_message>
updated gold/ orange, added Ashley K, fixed Taryn typo
</commit_message>
<xml_diff>
--- a/_site/data/DraftedTeams_Emails_Website.xlsx
+++ b/_site/data/DraftedTeams_Emails_Website.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="267">
   <si>
     <t>Team</t>
   </si>
@@ -803,13 +803,22 @@
   </si>
   <si>
     <t>iloveboogieboarding@gmail.com</t>
+  </si>
+  <si>
+    <t>Ashley King</t>
+  </si>
+  <si>
+    <t>King, Ashley</t>
+  </si>
+  <si>
+    <t>aking6@highpoint.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -828,13 +837,24 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FFE4E6EB"/>
+      <name val="&quot;Segoe UI Historic&quot;"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3E4042"/>
+        <bgColor rgb="FF3E4042"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -843,7 +863,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -869,6 +889,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2975,6 +2998,29 @@
         <v>18</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>